<commit_message>
Nova implementação - Informando data atual de teste realizado
</commit_message>
<xml_diff>
--- a/src/main/resources/ProjetoSI - Casos de teste - Funcionais Automatizados - E2E.xlsx
+++ b/src/main/resources/ProjetoSI - Casos de teste - Funcionais Automatizados - E2E.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">NOME DO TESTE AUTOMATIZADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA DE TESTE REALIZADO</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -167,6 +170,9 @@
     <t>FALHA: expected:&lt;...lterada com sucesso![S]&gt; but was:&lt;...lterada com sucesso![]&gt;</t>
   </si>
   <si>
+    <t>07/06/2023</t>
+  </si>
+  <si>
     <t>FALHA: expected:&lt;...cionada com sucesso![s]&gt; but was:&lt;...cionada com sucesso![]&gt;</t>
   </si>
   <si>
@@ -190,7 +196,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -239,6 +245,14 @@
     <font>
       <b val="true"/>
       <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -271,7 +285,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -300,6 +314,13 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -363,6 +384,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -377,10 +402,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -497,10 +518,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -508,15 +529,16 @@
     <col min="1" max="1" customWidth="true" hidden="false" style="0" width="4.5" collapsed="true" outlineLevel="0"/>
     <col min="2" max="2" customWidth="true" hidden="false" style="0" width="33.63" collapsed="true" outlineLevel="0"/>
     <col min="3" max="3" customWidth="true" hidden="false" style="0" width="35.38" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="31.27" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="31.28" collapsed="true" outlineLevel="0"/>
     <col min="5" max="5" customWidth="true" hidden="false" style="0" width="39.24" collapsed="true" outlineLevel="0"/>
     <col min="6" max="6" customWidth="true" hidden="false" style="0" width="22.62" collapsed="true" outlineLevel="0"/>
     <col min="7" max="7" customWidth="true" hidden="false" style="0" width="30.02" collapsed="true" outlineLevel="0"/>
     <col min="8" max="8" customWidth="true" hidden="false" style="0" width="44.46" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="1025" customWidth="true" hidden="false" style="0" width="12.63" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="0" width="32.96" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="1025" customWidth="true" hidden="false" style="0" width="12.63" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,163 +562,182 @@
       </c>
       <c r="H1" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="71.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="129.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>13</v>
+      <c r="E3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>20</v>
+        <v>48</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>13</v>
+      <c r="D5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>30</v>
+        <v>50</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="78.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>47</v>
+        <v>14</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="C7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="D7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="F7" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="G7" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="H7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C11">

</xml_diff>